<commit_message>
Tirei todos os prints dos arquivos e o relatorio final esta pronto
</commit_message>
<xml_diff>
--- a/transferencia.arquivos.tcp.udp.2019.xlsx
+++ b/transferencia.arquivos.tcp.udp.2019.xlsx
@@ -110,11 +110,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -360,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -557,10 +556,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,10 +564,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,19 +572,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,10 +593,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,10 +673,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G40"/>
+  <dimension ref="B1:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -745,7 +724,7 @@
         <v>11487307</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>11488</v>
+        <v>11534</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>4</v>
@@ -754,7 +733,7 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="n">
-        <v>5744</v>
+        <v>5756</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>5</v>
@@ -858,11 +837,18 @@
         <v>6</v>
       </c>
       <c r="D13" s="24" t="n">
-        <v>20</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="26"/>
+        <v>100</v>
+      </c>
+      <c r="E13" s="25" t="n">
+        <v>34.81</v>
+      </c>
+      <c r="F13" s="25" t="n">
+        <f aca="false">11.5/E13</f>
+        <v>0.330364837690319</v>
+      </c>
+      <c r="G13" s="26" t="n">
+        <v>5756</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="27" t="n">
@@ -872,109 +858,165 @@
         <v>4</v>
       </c>
       <c r="D14" s="28" t="n">
-        <v>20</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="30"/>
+        <v>100</v>
+      </c>
+      <c r="E14" s="29" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="F14" s="29" t="n">
+        <f aca="false">11.5/E14</f>
+        <v>0.237113402061856</v>
+      </c>
+      <c r="G14" s="30" t="n">
+        <v>5756</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="27" t="n">
         <v>2000</v>
       </c>
       <c r="C15" s="28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="28" t="n">
-        <v>40</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="30"/>
+        <v>100</v>
+      </c>
+      <c r="E15" s="29" t="n">
+        <v>80.6</v>
+      </c>
+      <c r="F15" s="29" t="n">
+        <f aca="false">11.5/E15</f>
+        <v>0.142679900744417</v>
+      </c>
+      <c r="G15" s="30" t="n">
+        <v>5756</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="27" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C16" s="28" t="n">
         <v>6</v>
       </c>
       <c r="D16" s="28" t="n">
-        <v>40</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="30"/>
+        <v>100</v>
+      </c>
+      <c r="E16" s="29" t="n">
+        <v>80.4</v>
+      </c>
+      <c r="F16" s="29" t="n">
+        <f aca="false">11.5/E16</f>
+        <v>0.143034825870647</v>
+      </c>
+      <c r="G16" s="30" t="n">
+        <v>5756</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="27" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C17" s="28" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17" s="28" t="n">
-        <v>20</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="30"/>
+        <v>100</v>
+      </c>
+      <c r="E17" s="29" t="n">
+        <v>96.5</v>
+      </c>
+      <c r="F17" s="29" t="n">
+        <f aca="false">11.5/E17</f>
+        <v>0.119170984455959</v>
+      </c>
+      <c r="G17" s="30" t="n">
+        <v>5756</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="31" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C18" s="32" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="32" t="n">
-        <v>40</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="34"/>
+        <v>100</v>
+      </c>
+      <c r="E18" s="33" t="n">
+        <v>161.7</v>
+      </c>
+      <c r="F18" s="33" t="n">
+        <f aca="false">11.5/E18</f>
+        <v>0.0711193568336426</v>
+      </c>
+      <c r="G18" s="34" t="n">
+        <v>5756</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C19" s="36" t="n">
         <v>6</v>
       </c>
       <c r="D19" s="36" t="n">
-        <v>20</v>
-      </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="38"/>
+        <v>200</v>
+      </c>
+      <c r="E19" s="37" t="n">
+        <v>34.8</v>
+      </c>
+      <c r="F19" s="37" t="n">
+        <f aca="false">11.5/E19</f>
+        <v>0.330459770114943</v>
+      </c>
+      <c r="G19" s="38" t="n">
+        <v>11534</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="39" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C20" s="40" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="40" t="n">
-        <v>40</v>
-      </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="42"/>
+        <v>200</v>
+      </c>
+      <c r="E20" s="41" t="n">
+        <v>48.7</v>
+      </c>
+      <c r="F20" s="41" t="n">
+        <f aca="false">11.5/E20</f>
+        <v>0.236139630390144</v>
+      </c>
+      <c r="G20" s="42" t="n">
+        <v>11534</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="39" t="n">
         <v>1000</v>
       </c>
       <c r="C21" s="40" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21" s="40" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="42"/>
+        <v>200</v>
+      </c>
+      <c r="E21" s="41" t="n">
+        <v>69.8</v>
+      </c>
+      <c r="F21" s="41" t="n">
+        <f aca="false">11.5/E21</f>
+        <v>0.164756446991404</v>
+      </c>
+      <c r="G21" s="42" t="n">
+        <v>11534</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="39" t="n">
@@ -984,25 +1026,39 @@
         <v>4</v>
       </c>
       <c r="D22" s="40" t="n">
-        <v>40</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="42"/>
+        <v>200</v>
+      </c>
+      <c r="E22" s="41" t="n">
+        <v>97.3</v>
+      </c>
+      <c r="F22" s="41" t="n">
+        <f aca="false">11.5/E22</f>
+        <v>0.118191161356629</v>
+      </c>
+      <c r="G22" s="42" t="n">
+        <v>11534</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="39" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C23" s="40" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="40" t="n">
-        <v>20</v>
-      </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="42"/>
+        <v>200</v>
+      </c>
+      <c r="E23" s="41" t="n">
+        <v>80.6</v>
+      </c>
+      <c r="F23" s="41" t="n">
+        <f aca="false">11.5/E23</f>
+        <v>0.142679900744417</v>
+      </c>
+      <c r="G23" s="42" t="n">
+        <v>11534</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="43" t="n">
@@ -1012,13 +1068,20 @@
         <v>2</v>
       </c>
       <c r="D24" s="44" t="n">
-        <v>40</v>
-      </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="46"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>200</v>
+      </c>
+      <c r="E24" s="45" t="n">
+        <v>161.8</v>
+      </c>
+      <c r="F24" s="45" t="n">
+        <f aca="false">11.5/E24</f>
+        <v>0.0710754017305315</v>
+      </c>
+      <c r="G24" s="46" t="n">
+        <v>11534</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="0"/>
       <c r="C26" s="0"/>
@@ -1055,112 +1118,155 @@
       <c r="D29" s="48" t="n">
         <v>100</v>
       </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="E29" s="25" t="n">
+        <v>18.7615384615385</v>
+      </c>
+      <c r="F29" s="25" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="G29" s="26" t="n">
+        <v>5756</v>
+      </c>
+      <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="50" t="n">
+      <c r="B30" s="49" t="n">
         <v>2000</v>
       </c>
-      <c r="C30" s="51" t="n">
+      <c r="C30" s="50" t="n">
         <v>4</v>
       </c>
-      <c r="D30" s="51" t="n">
+      <c r="D30" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
+      <c r="E30" s="29" t="n">
+        <v>18.5538461538462</v>
+      </c>
+      <c r="F30" s="29" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G30" s="30" t="n">
+        <v>5756</v>
+      </c>
+      <c r="I30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="50" t="n">
+      <c r="B31" s="49" t="n">
         <v>2000</v>
       </c>
-      <c r="C31" s="51" t="n">
+      <c r="C31" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="D31" s="51" t="n">
+      <c r="D31" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="E31" s="52"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="E31" s="29" t="n">
+        <v>16.8461538461538</v>
+      </c>
+      <c r="F31" s="29" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G31" s="30" t="n">
+        <v>5756</v>
+      </c>
+      <c r="I31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="53" t="n">
+      <c r="B32" s="51" t="n">
         <v>1000</v>
       </c>
-      <c r="C32" s="54" t="n">
+      <c r="C32" s="52" t="n">
         <v>6</v>
       </c>
-      <c r="D32" s="54" t="n">
+      <c r="D32" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
+      <c r="E32" s="41" t="n">
+        <v>19.9384615384615</v>
+      </c>
+      <c r="F32" s="41" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G32" s="42" t="n">
+        <v>11534</v>
+      </c>
+      <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="53" t="n">
+      <c r="B33" s="51" t="n">
         <v>1000</v>
       </c>
-      <c r="C33" s="54" t="n">
+      <c r="C33" s="52" t="n">
         <v>4</v>
       </c>
-      <c r="D33" s="54" t="n">
+      <c r="D33" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="E33" s="55"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
+      <c r="E33" s="41" t="n">
+        <v>20.4615384615385</v>
+      </c>
+      <c r="F33" s="41" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G33" s="42" t="n">
+        <v>11534</v>
+      </c>
+      <c r="I33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="53" t="n">
+      <c r="B34" s="51" t="n">
         <v>1000</v>
       </c>
-      <c r="C34" s="54" t="n">
+      <c r="C34" s="52" t="n">
         <v>2</v>
       </c>
-      <c r="D34" s="54" t="n">
+      <c r="D34" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="E34" s="55"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
+      <c r="E34" s="41" t="n">
+        <v>21.3461538461538</v>
+      </c>
+      <c r="F34" s="41" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G34" s="42" t="n">
+        <v>11534</v>
+      </c>
+      <c r="I34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="56" t="n">
+      <c r="B35" s="53" t="n">
         <v>2000</v>
       </c>
-      <c r="C35" s="57" t="n">
+      <c r="C35" s="54" t="n">
         <v>6</v>
       </c>
-      <c r="D35" s="57" t="n">
+      <c r="D35" s="54" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="58" t="n">
-        <v>55.6</v>
-      </c>
-      <c r="F35" s="59" t="n">
+      <c r="E35" s="55" t="n">
+        <v>21.3846153846154</v>
+      </c>
+      <c r="F35" s="55" t="n">
         <v>0.28</v>
       </c>
-      <c r="G35" s="60" t="n">
+      <c r="G35" s="56" t="n">
         <v>5756</v>
       </c>
+      <c r="I35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="50" t="n">
+      <c r="B36" s="49" t="n">
         <v>2000</v>
       </c>
-      <c r="C36" s="51" t="n">
+      <c r="C36" s="50" t="n">
         <v>4</v>
       </c>
-      <c r="D36" s="51" t="n">
+      <c r="D36" s="50" t="n">
         <v>200</v>
       </c>
-      <c r="E36" s="52" t="n">
-        <v>52.8</v>
+      <c r="E36" s="29" t="n">
+        <v>20.3076923076923</v>
       </c>
       <c r="F36" s="29" t="n">
         <v>0.217</v>
@@ -1168,62 +1274,91 @@
       <c r="G36" s="30" t="n">
         <v>5756</v>
       </c>
+      <c r="I36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="53" t="n">
+      <c r="B37" s="51" t="n">
         <v>1000</v>
       </c>
-      <c r="C37" s="54" t="n">
+      <c r="C37" s="52" t="n">
         <v>6</v>
       </c>
-      <c r="D37" s="54" t="n">
+      <c r="D37" s="52" t="n">
         <v>200</v>
       </c>
-      <c r="E37" s="55"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="42"/>
+      <c r="E37" s="41" t="n">
+        <v>20.3076923076923</v>
+      </c>
+      <c r="F37" s="41" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G37" s="42" t="n">
+        <v>11534</v>
+      </c>
+      <c r="I37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="53" t="n">
+      <c r="B38" s="51" t="n">
         <v>1000</v>
       </c>
-      <c r="C38" s="54" t="n">
+      <c r="C38" s="52" t="n">
         <v>4</v>
       </c>
-      <c r="D38" s="54" t="n">
+      <c r="D38" s="52" t="n">
         <v>200</v>
       </c>
-      <c r="E38" s="55"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="42"/>
+      <c r="E38" s="41" t="n">
+        <v>19.4615384615385</v>
+      </c>
+      <c r="F38" s="41" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G38" s="42" t="n">
+        <v>11534</v>
+      </c>
+      <c r="I38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="50" t="n">
+      <c r="B39" s="49" t="n">
         <v>2000</v>
       </c>
-      <c r="C39" s="51" t="n">
+      <c r="C39" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="D39" s="51" t="n">
+      <c r="D39" s="50" t="n">
         <v>200</v>
       </c>
-      <c r="E39" s="52"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="30"/>
+      <c r="E39" s="29" t="n">
+        <v>22.9615384615385</v>
+      </c>
+      <c r="F39" s="29" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G39" s="30" t="n">
+        <v>5756</v>
+      </c>
+      <c r="I39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="61" t="n">
+      <c r="B40" s="57" t="n">
         <v>1000</v>
       </c>
-      <c r="C40" s="62" t="n">
+      <c r="C40" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="D40" s="62" t="n">
+      <c r="D40" s="58" t="n">
         <v>200</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="46"/>
+      <c r="E40" s="45" t="n">
+        <v>27.0961538461538</v>
+      </c>
+      <c r="F40" s="45" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="G40" s="46" t="n">
+        <v>11534</v>
+      </c>
+      <c r="I40" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>